<commit_message>
developed binary classifiers using data for all 6 ligand-receptor complex types, removed GPR31 classification code from copied notebooks
</commit_message>
<xml_diff>
--- a/model_performance_comparison.xlsx
+++ b/model_performance_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://livememphis-my.sharepoint.com/personal/gszwbwsk_memphis_edu/Documents/Machine Learning/GPCR_DB_project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="910" documentId="11_F25DC773A252ABDACC10485D395E5B1C5ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{421AC8C1-5F0F-4521-96B9-3CA5534AC2DD}"/>
+  <xr:revisionPtr revIDLastSave="1023" documentId="11_F25DC773A252ABDACC10485D395E5B1C5ADE58E7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32E17684-A8DB-4D32-81B8-687394FA986D}"/>
   <bookViews>
-    <workbookView xWindow="22680" yWindow="3255" windowWidth="16665" windowHeight="11475" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21735" yWindow="3255" windowWidth="7065" windowHeight="11475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pre gridsearch" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="51">
   <si>
     <t>Residues Dropped</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>HM inactives</t>
+  </si>
+  <si>
+    <t>LM_binary</t>
+  </si>
+  <si>
+    <t>noLM_binary</t>
   </si>
 </sst>
 </file>
@@ -528,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R20"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,70 +970,340 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9">
+        <v>1000</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9">
+        <v>0.86</v>
+      </c>
+      <c r="J9">
+        <v>0.86</v>
+      </c>
+      <c r="K9">
+        <v>0.86</v>
+      </c>
+      <c r="L9">
+        <v>0.86</v>
+      </c>
+      <c r="M9" s="2">
+        <v>100</v>
+      </c>
+      <c r="N9" s="2">
+        <v>90.91</v>
+      </c>
+      <c r="O9" s="2">
+        <v>100</v>
+      </c>
+      <c r="P9" s="2">
+        <v>98.7</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>63.8</v>
+      </c>
+      <c r="R9" s="2">
+        <v>54.69</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
+      <c r="A10" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10">
+        <v>1000</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0.79</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0.76</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0.76</v>
+      </c>
+      <c r="M10" s="2">
+        <v>97.78</v>
+      </c>
+      <c r="N10" s="2">
+        <v>45.45</v>
+      </c>
+      <c r="O10" s="2">
+        <v>98.68</v>
+      </c>
+      <c r="P10" s="2">
+        <v>97.47</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>71.25</v>
+      </c>
+      <c r="R10" s="2">
+        <v>32.81</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
+      <c r="A11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11">
+        <v>1000</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0.87</v>
+      </c>
+      <c r="M11" s="2">
+        <v>100</v>
+      </c>
+      <c r="N11" s="2">
+        <v>96.97</v>
+      </c>
+      <c r="O11" s="2">
+        <v>100</v>
+      </c>
+      <c r="P11" s="2">
+        <v>100</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>67.5</v>
+      </c>
+      <c r="R11" s="2">
+        <v>53.12</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
+      <c r="A12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12">
+        <v>1000</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="K12" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="M12" s="2">
+        <v>98.89</v>
+      </c>
+      <c r="N12" s="2">
+        <v>87.88</v>
+      </c>
+      <c r="O12" s="2">
+        <v>100</v>
+      </c>
+      <c r="P12" s="2">
+        <v>97.47</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>68.75</v>
+      </c>
+      <c r="R12" s="2">
+        <v>50</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
+      <c r="A13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13">
+        <v>1000</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="M13" s="2">
+        <v>95.56</v>
+      </c>
+      <c r="N13" s="2">
+        <v>54.55</v>
+      </c>
+      <c r="O13" s="2">
+        <v>98.68</v>
+      </c>
+      <c r="P13" s="2">
+        <v>97.47</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>72.5</v>
+      </c>
+      <c r="R13" s="2">
+        <v>28.12</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14">
+        <v>1000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.86</v>
+      </c>
+      <c r="M14" s="2">
+        <v>100</v>
+      </c>
+      <c r="N14" s="2">
+        <v>95.45</v>
+      </c>
+      <c r="O14" s="2">
+        <v>100</v>
+      </c>
+      <c r="P14" s="2">
+        <v>100</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>73.75</v>
+      </c>
+      <c r="R14" s="2">
+        <v>37.5</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I15" s="2"/>
@@ -1109,14 +1385,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B42B8B0B-B6E3-4D15-B12D-5D71BF49680D}">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3:Q8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
@@ -1326,7 +1603,7 @@
         <v>82.3</v>
       </c>
       <c r="Q4">
-        <f t="shared" ref="Q4:Q8" si="0">AVERAGE(M4:P4)</f>
+        <f t="shared" ref="Q4:Q10" si="0">AVERAGE(M4:P4)</f>
         <v>79</v>
       </c>
       <c r="R4">
@@ -1574,6 +1851,126 @@
       </c>
       <c r="S8">
         <v>89.1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9">
+        <v>1000</v>
+      </c>
+      <c r="D9" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>30</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>2</v>
+      </c>
+      <c r="I9">
+        <v>0.9</v>
+      </c>
+      <c r="J9">
+        <v>0.88</v>
+      </c>
+      <c r="K9">
+        <v>0.88</v>
+      </c>
+      <c r="L9">
+        <v>0.88</v>
+      </c>
+      <c r="M9">
+        <v>100</v>
+      </c>
+      <c r="N9">
+        <v>96.97</v>
+      </c>
+      <c r="O9">
+        <v>100</v>
+      </c>
+      <c r="P9">
+        <v>100</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="0"/>
+        <v>99.242500000000007</v>
+      </c>
+      <c r="R9">
+        <v>77.5</v>
+      </c>
+      <c r="S9">
+        <v>46.88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10">
+        <v>1000</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>5</v>
+      </c>
+      <c r="I10">
+        <v>0.9</v>
+      </c>
+      <c r="J10">
+        <v>0.85</v>
+      </c>
+      <c r="K10">
+        <v>0.84</v>
+      </c>
+      <c r="L10">
+        <v>0.85</v>
+      </c>
+      <c r="M10">
+        <v>100</v>
+      </c>
+      <c r="N10">
+        <v>95.45</v>
+      </c>
+      <c r="O10">
+        <v>100</v>
+      </c>
+      <c r="P10">
+        <v>100</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>98.862499999999997</v>
+      </c>
+      <c r="R10">
+        <v>58.75</v>
+      </c>
+      <c r="S10">
+        <v>46.88</v>
       </c>
     </row>
   </sheetData>
@@ -3949,7 +4346,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF287CA-4628-41A2-AAE7-5B3FBED99A28}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>